<commit_message>
Nhan Nguyen added Data for .R file
</commit_message>
<xml_diff>
--- a/6. Coding and documentation/Data/Eurostat_employment_isco.xlsx
+++ b/6. Coding and documentation/Data/Eurostat_employment_isco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whard\OneDrive\Desktop\Reproducible research\Recoding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UW\2. Summer 22-23\5. Reproducible Research\RRcourse2023\6. Coding and documentation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BEFDF46-A361-48D8-9834-62D13AAA7D9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9A0549-520C-43F4-AC72-6BCBDA65E23F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21732" windowHeight="5940" xr2:uid="{AB8E089C-3C03-4BA6-B14E-D8632E128822}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{AB8E089C-3C03-4BA6-B14E-D8632E128822}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
@@ -40,6 +40,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -208,11 +217,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.##########"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,15 +237,33 @@
       <sz val="9"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -283,10 +313,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -315,9 +346,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -333,9 +384,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -373,7 +424,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -479,7 +530,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -629,15 +680,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38363672-59F0-4595-8DCF-6E865AA04F3A}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.86328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,8 +724,19 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -706,8 +770,19 @@
       <c r="K2" s="4">
         <v>4406.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M2" s="16"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -741,8 +816,19 @@
       <c r="K3" s="4">
         <v>4519.3999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M3" s="16"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="19"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -776,8 +862,19 @@
       <c r="K4" s="4">
         <v>4578.8999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M4" s="16"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -811,8 +908,19 @@
       <c r="K5" s="4">
         <v>4487.8999999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M5" s="16"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -846,8 +954,19 @@
       <c r="K6" s="4">
         <v>4428.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M6" s="16"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -881,8 +1000,19 @@
       <c r="K7" s="4">
         <v>4531.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M7" s="16"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -916,8 +1046,19 @@
       <c r="K8" s="6">
         <v>4585</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M8" s="16"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -951,8 +1092,19 @@
       <c r="K9" s="4">
         <v>4493.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M9" s="16"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -986,8 +1138,19 @@
       <c r="K10" s="4">
         <v>4460.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M10" s="16"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -1021,8 +1184,19 @@
       <c r="K11" s="4">
         <v>4564.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M11" s="16"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -1056,8 +1230,19 @@
       <c r="K12" s="4">
         <v>4637.6000000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M12" s="16"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -1091,8 +1276,19 @@
       <c r="K13" s="4">
         <v>4554.7</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M13" s="16"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -1126,8 +1322,19 @@
       <c r="K14" s="4">
         <v>4499.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M14" s="16"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="19"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -1161,8 +1368,19 @@
       <c r="K15" s="4">
         <v>4603.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M15" s="16"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -1196,8 +1414,19 @@
       <c r="K16" s="4">
         <v>4698.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M16" s="16"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -1231,8 +1460,19 @@
       <c r="K17" s="4">
         <v>4588.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M17" s="16"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -1266,8 +1506,19 @@
       <c r="K18" s="4">
         <v>4559.3999999999996</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M18" s="16"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="18"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -1301,8 +1552,19 @@
       <c r="K19" s="4">
         <v>4658.8999999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M19" s="16"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="19"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -1336,8 +1598,19 @@
       <c r="K20" s="4">
         <v>4744.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M20" s="16"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="18"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -1371,8 +1644,19 @@
       <c r="K21" s="4">
         <v>4676.8999999999996</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M21" s="16"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -1406,8 +1690,19 @@
       <c r="K22" s="6">
         <v>4638</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M22" s="16"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="19"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -1441,8 +1736,19 @@
       <c r="K23" s="4">
         <v>4755.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M23" s="16"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="19"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -1476,8 +1782,19 @@
       <c r="K24" s="4">
         <v>4806.3999999999996</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M24" s="16"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -1511,8 +1828,19 @@
       <c r="K25" s="4">
         <v>4742.7</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M25" s="16"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -1546,8 +1874,19 @@
       <c r="K26" s="4">
         <v>4745.1000000000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M26" s="16"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="18"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -1581,8 +1920,19 @@
       <c r="K27" s="4">
         <v>4842.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M27" s="16"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -1616,8 +1966,19 @@
       <c r="K28" s="4">
         <v>4912.8</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M28" s="16"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="18"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -1651,8 +2012,19 @@
       <c r="K29" s="4">
         <v>4834.8999999999996</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M29" s="16"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -1686,8 +2058,19 @@
       <c r="K30" s="4">
         <v>4823.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M30" s="16"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -1721,8 +2104,19 @@
       <c r="K31" s="4">
         <v>4928.8999999999996</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M31" s="16"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="19"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -1756,8 +2150,19 @@
       <c r="K32" s="4">
         <v>4985.1000000000004</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M32" s="16"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -1791,8 +2196,19 @@
       <c r="K33" s="4">
         <v>4903.3999999999996</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M33" s="16"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -1826,8 +2242,19 @@
       <c r="K34" s="4">
         <v>4864.2</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M34" s="16"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -1861,8 +2288,19 @@
       <c r="K35" s="4">
         <v>4954.8999999999996</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M35" s="16"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="18"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -1896,8 +2334,19 @@
       <c r="K36" s="6">
         <v>5006</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M36" s="16"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="19"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -1931,8 +2380,19 @@
       <c r="K37" s="4">
         <v>4928.8999999999996</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M37" s="16"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -1966,8 +2426,19 @@
       <c r="K38" s="4">
         <v>4849.3999999999996</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M38" s="16"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -2001,8 +2472,19 @@
       <c r="K39" s="4">
         <v>4846.3</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M39" s="16"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="19"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -2036,8 +2518,19 @@
       <c r="K40" s="4">
         <v>4897.1000000000004</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M40" s="16"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -2071,8 +2564,36 @@
       <c r="K41" s="4">
         <v>4857.6000000000004</v>
       </c>
+      <c r="M41" s="16"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="18"/>
+      <c r="W41" s="19"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="N42" s="10">
+        <f>SUM(N2:N41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="N43" s="12">
+        <f>N42*9</f>
+        <v>0</v>
+      </c>
+      <c r="O43" s="4"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="O44" s="11"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K41" xr:uid="{DFEB4528-6931-4975-A20C-88184FF5D33B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2082,12 +2603,12 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2122,7 +2643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -2157,7 +2678,7 @@
         <v>220.6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -2192,7 +2713,7 @@
         <v>240.8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -2227,7 +2748,7 @@
         <v>244.8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -2262,7 +2783,7 @@
         <v>231.2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -2297,7 +2818,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -2332,7 +2853,7 @@
         <v>235.4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -2367,7 +2888,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -2402,7 +2923,7 @@
         <v>223.6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -2437,7 +2958,7 @@
         <v>222.8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -2472,7 +2993,7 @@
         <v>234.8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -2507,7 +3028,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -2542,7 +3063,7 @@
         <v>237.1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -2577,7 +3098,7 @@
         <v>224.3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -2612,7 +3133,7 @@
         <v>234.7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -2647,7 +3168,7 @@
         <v>251.4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -2682,7 +3203,7 @@
         <v>226.4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -2717,7 +3238,7 @@
         <v>221.1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -2752,7 +3273,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -2787,7 +3308,7 @@
         <v>237.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -2822,7 +3343,7 @@
         <v>230.1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -2857,7 +3378,7 @@
         <v>218.6</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -2892,7 +3413,7 @@
         <v>228.1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -2927,7 +3448,7 @@
         <v>239.9</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -2962,7 +3483,7 @@
         <v>231.7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -2997,7 +3518,7 @@
         <v>230.4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -3032,7 +3553,7 @@
         <v>230.5</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -3067,7 +3588,7 @@
         <v>238.4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -3102,7 +3623,7 @@
         <v>224.9</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -3137,7 +3658,7 @@
         <v>221.1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -3172,7 +3693,7 @@
         <v>237.5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -3207,7 +3728,7 @@
         <v>246.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -3242,7 +3763,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -3277,7 +3798,7 @@
         <v>226.9</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -3312,7 +3833,7 @@
         <v>238.7</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -3347,7 +3868,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -3382,7 +3903,7 @@
         <v>217.4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -3417,7 +3938,7 @@
         <v>217.5</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -3452,7 +3973,7 @@
         <v>210.3</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -3487,7 +4008,7 @@
         <v>218.5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -3532,12 +4053,15 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="24.3984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3572,7 +4096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -3607,7 +4131,7 @@
         <v>232.6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -3642,7 +4166,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -3677,7 +4201,7 @@
         <v>238.5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -3712,7 +4236,7 @@
         <v>246.1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -3747,7 +4271,7 @@
         <v>249.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -3782,7 +4306,7 @@
         <v>260.7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -3817,7 +4341,7 @@
         <v>266.10000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -3852,7 +4376,7 @@
         <v>265.60000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -3887,7 +4411,7 @@
         <v>265.39999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -3922,7 +4446,7 @@
         <v>257.3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -3957,7 +4481,7 @@
         <v>265.10000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -3992,7 +4516,7 @@
         <v>261.7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -4027,7 +4551,7 @@
         <v>260.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -4062,7 +4586,7 @@
         <v>257.7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -4097,7 +4621,7 @@
         <v>254.2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -4132,7 +4656,7 @@
         <v>251.8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -4167,7 +4691,7 @@
         <v>253.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -4202,7 +4726,7 @@
         <v>260.5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -4237,7 +4761,7 @@
         <v>259.89999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -4272,7 +4796,7 @@
         <v>270.7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -4307,7 +4831,7 @@
         <v>267.89999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -4342,7 +4866,7 @@
         <v>272.5</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -4377,7 +4901,7 @@
         <v>290.60000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -4412,7 +4936,7 @@
         <v>279.60000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -4447,7 +4971,7 @@
         <v>284.5</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -4482,7 +5006,7 @@
         <v>286.2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -4517,7 +5041,7 @@
         <v>288.7</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -4552,7 +5076,7 @@
         <v>299.10000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -4587,7 +5111,7 @@
         <v>302.89999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -4622,7 +5146,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -4657,7 +5181,7 @@
         <v>297.7</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -4692,7 +5216,7 @@
         <v>310.5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -4727,7 +5251,7 @@
         <v>300.39999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -4762,7 +5286,7 @@
         <v>313.7</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -4797,7 +5321,7 @@
         <v>315.39999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -4832,7 +5356,7 @@
         <v>312.89999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -4867,7 +5391,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -4902,7 +5426,7 @@
         <v>309.5</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -4937,7 +5461,7 @@
         <v>311.5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -4981,13 +5505,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CD73FB-C105-4354-9D07-596E10C310F1}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5022,7 +5546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -5057,7 +5581,7 @@
         <v>1102.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -5092,7 +5616,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -5127,7 +5651,7 @@
         <v>1125.4000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -5162,7 +5686,7 @@
         <v>1131.2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -5197,7 +5721,7 @@
         <v>1135.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -5232,7 +5756,7 @@
         <v>1135.5999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -5267,7 +5791,7 @@
         <v>1127.7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -5302,7 +5826,7 @@
         <v>1144.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -5337,7 +5861,7 @@
         <v>1144.8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -5372,7 +5896,7 @@
         <v>1161.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -5407,7 +5931,7 @@
         <v>1160.5999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -5442,7 +5966,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -5477,7 +6001,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -5512,7 +6036,7 @@
         <v>1193.3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -5547,7 +6071,7 @@
         <v>1202.7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -5582,7 +6106,7 @@
         <v>1217.8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -5617,7 +6141,7 @@
         <v>1222.5999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -5652,7 +6176,7 @@
         <v>1237.5999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -5687,7 +6211,7 @@
         <v>1248.5999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -5722,7 +6246,7 @@
         <v>1261.4000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -5757,7 +6281,7 @@
         <v>1276.4000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -5792,7 +6316,7 @@
         <v>1314.6</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -5827,7 +6351,7 @@
         <v>1325.5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -5862,7 +6386,7 @@
         <v>1327.2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -5897,7 +6421,7 @@
         <v>1325.9</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -5932,7 +6456,7 @@
         <v>1342.2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -5967,7 +6491,7 @@
         <v>1351.9</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -6002,7 +6526,7 @@
         <v>1362.6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -6037,7 +6561,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -6072,7 +6596,7 @@
         <v>1408.9</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -6107,7 +6631,7 @@
         <v>1424.4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -6142,7 +6666,7 @@
         <v>1421.8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -6177,7 +6701,7 @@
         <v>1445.3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -6212,7 +6736,7 @@
         <v>1471.2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -6247,7 +6771,7 @@
         <v>1475.5</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -6282,7 +6806,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -6317,7 +6841,7 @@
         <v>1489.4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -6352,7 +6876,7 @@
         <v>1502.2</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -6387,7 +6911,7 @@
         <v>1495.9</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -6432,12 +6956,12 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6472,7 +6996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -6507,7 +7031,7 @@
         <v>722.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -6542,7 +7066,7 @@
         <v>722.3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -6577,7 +7101,7 @@
         <v>730.2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -6612,7 +7136,7 @@
         <v>733.9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -6647,7 +7171,7 @@
         <v>731.7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -6682,7 +7206,7 @@
         <v>740.9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -6717,7 +7241,7 @@
         <v>745.1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -6752,7 +7276,7 @@
         <v>760.2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -6787,7 +7311,7 @@
         <v>762.5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -6822,7 +7346,7 @@
         <v>775.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -6857,7 +7381,7 @@
         <v>779.8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -6892,7 +7416,7 @@
         <v>788.2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -6927,7 +7451,7 @@
         <v>793.7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -6962,7 +7486,7 @@
         <v>805.2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -6997,7 +7521,7 @@
         <v>818.3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -7032,7 +7556,7 @@
         <v>812.3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -7067,7 +7591,7 @@
         <v>831.9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -7102,7 +7626,7 @@
         <v>828.8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -7137,7 +7661,7 @@
         <v>831.5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -7172,7 +7696,7 @@
         <v>843.1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -7207,7 +7731,7 @@
         <v>858.1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -7242,7 +7766,7 @@
         <v>862.8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -7277,7 +7801,7 @@
         <v>858.7</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -7312,7 +7836,7 @@
         <v>855.8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -7347,7 +7871,7 @@
         <v>871.2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -7382,7 +7906,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -7417,7 +7941,7 @@
         <v>902.2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -7452,7 +7976,7 @@
         <v>891.6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -7487,7 +8011,7 @@
         <v>902.4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -7522,7 +8046,7 @@
         <v>913.9</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -7557,7 +8081,7 @@
         <v>914.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -7592,7 +8116,7 @@
         <v>908.4</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -7627,7 +8151,7 @@
         <v>904.7</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -7662,7 +8186,7 @@
         <v>897.4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -7697,7 +8221,7 @@
         <v>907.3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -7732,7 +8256,7 @@
         <v>927.8</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -7767,7 +8291,7 @@
         <v>922.2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -7802,7 +8326,7 @@
         <v>904.8</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -7837,7 +8361,7 @@
         <v>923.2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -7882,12 +8406,12 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7922,7 +8446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -7957,7 +8481,7 @@
         <v>267.3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -7992,7 +8516,7 @@
         <v>275.10000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -8027,7 +8551,7 @@
         <v>271.89999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -8062,7 +8586,7 @@
         <v>264.8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -8097,7 +8621,7 @@
         <v>261.10000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -8132,7 +8656,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -8167,7 +8691,7 @@
         <v>268.89999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -8202,7 +8726,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -8237,7 +8761,7 @@
         <v>261.3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -8272,7 +8796,7 @@
         <v>273.2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -8307,7 +8831,7 @@
         <v>279.2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -8342,7 +8866,7 @@
         <v>267.39999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -8377,7 +8901,7 @@
         <v>261.60000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -8412,7 +8936,7 @@
         <v>273.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -8447,7 +8971,7 @@
         <v>291.89999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -8482,7 +9006,7 @@
         <v>276.60000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -8517,7 +9041,7 @@
         <v>277.2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -8552,7 +9076,7 @@
         <v>290.10000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -8587,7 +9111,7 @@
         <v>310.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -8622,7 +9146,7 @@
         <v>308.3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -8657,7 +9181,7 @@
         <v>302.60000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -8692,7 +9216,7 @@
         <v>300.60000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -8727,7 +9251,7 @@
         <v>304.39999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -8762,7 +9286,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -8797,7 +9321,7 @@
         <v>299.10000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -8832,7 +9356,7 @@
         <v>315.5</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -8867,7 +9391,7 @@
         <v>322.60000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -8902,7 +9426,7 @@
         <v>309.39999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -8937,7 +9461,7 @@
         <v>310.8</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -8972,7 +9496,7 @@
         <v>310.39999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -9007,7 +9531,7 @@
         <v>307.7</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -9042,7 +9566,7 @@
         <v>313.8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -9077,7 +9601,7 @@
         <v>287.5</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -9112,7 +9636,7 @@
         <v>287.89999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -9147,7 +9671,7 @@
         <v>293.5</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -9182,7 +9706,7 @@
         <v>294.2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -9217,7 +9741,7 @@
         <v>269.39999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -9252,7 +9776,7 @@
         <v>282.7</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -9287,7 +9811,7 @@
         <v>291.2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -9329,16 +9853,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA20AC9-EAA9-43DD-8DD7-3B4A74C3BB15}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD81"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9373,7 +9896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -9408,7 +9931,7 @@
         <v>920.7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -9443,7 +9966,7 @@
         <v>956.6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -9478,7 +10001,7 @@
         <v>984.3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -9513,7 +10036,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -9548,7 +10071,7 @@
         <v>916.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -9583,7 +10106,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -9618,7 +10141,7 @@
         <v>976.3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -9653,7 +10176,7 @@
         <v>916.2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -9688,7 +10211,7 @@
         <v>908.4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -9723,7 +10246,7 @@
         <v>938.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -9758,7 +10281,7 @@
         <v>966.6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -9793,7 +10316,7 @@
         <v>919.4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -9828,7 +10351,7 @@
         <v>908.1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -9863,7 +10386,7 @@
         <v>932.2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -9898,7 +10421,7 @@
         <v>971.3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -9933,7 +10456,7 @@
         <v>919.7</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -9968,7 +10491,7 @@
         <v>899.2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -10003,7 +10526,7 @@
         <v>940.3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -10038,7 +10561,7 @@
         <v>962.9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -10073,7 +10596,7 @@
         <v>905.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -10108,7 +10631,7 @@
         <v>889.1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -10143,7 +10666,7 @@
         <v>933.3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -10178,7 +10701,7 @@
         <v>940.6</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -10213,7 +10736,7 @@
         <v>920.9</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -10248,7 +10771,7 @@
         <v>918.5</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -10283,7 +10806,7 @@
         <v>952.5</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -10318,7 +10841,7 @@
         <v>964.3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -10353,7 +10876,7 @@
         <v>932.7</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -10388,7 +10911,7 @@
         <v>901.4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -10423,7 +10946,7 @@
         <v>930.8</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -10458,7 +10981,7 @@
         <v>940.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -10493,7 +11016,7 @@
         <v>890.8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -10528,7 +11051,7 @@
         <v>885.7</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -10563,7 +11086,7 @@
         <v>917.6</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -10598,7 +11121,7 @@
         <v>925.4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -10633,7 +11156,7 @@
         <v>879.7</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -10668,7 +11191,7 @@
         <v>857.3</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -10703,7 +11226,7 @@
         <v>845.9</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -10738,7 +11261,7 @@
         <v>854.7</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -10774,11 +11297,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K41" xr:uid="{8C5CB4E7-3900-4EC4-AFC5-84CDEE4C2434}">
-    <filterColumn colId="0">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K41" xr:uid="{8C5CB4E7-3900-4EC4-AFC5-84CDEE4C2434}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10788,12 +11307,12 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10828,7 +11347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -10863,7 +11382,7 @@
         <v>66.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -10898,7 +11417,7 @@
         <v>73.900000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -10933,7 +11452,7 @@
         <v>75.599999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -10968,7 +11487,7 @@
         <v>69.099999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -11003,7 +11522,7 @@
         <v>68.400000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -11038,7 +11557,7 @@
         <v>75.400000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -11073,7 +11592,7 @@
         <v>76.8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -11108,7 +11627,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -11143,7 +11662,7 @@
         <v>63.8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -11178,7 +11697,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -11213,7 +11732,7 @@
         <v>77.3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -11248,7 +11767,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -11283,7 +11802,7 @@
         <v>60.9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -11318,7 +11837,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -11353,7 +11872,7 @@
         <v>78.3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -11388,7 +11907,7 @@
         <v>64.400000000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -11423,7 +11942,7 @@
         <v>64.599999999999994</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -11458,7 +11977,7 @@
         <v>77.400000000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -11493,7 +12012,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -11528,7 +12047,7 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -11563,7 +12082,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -11598,7 +12117,7 @@
         <v>74.900000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -11633,7 +12152,7 @@
         <v>79.7</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -11668,7 +12187,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -11703,7 +12222,7 @@
         <v>64.900000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -11738,7 +12257,7 @@
         <v>71.2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -11773,7 +12292,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -11808,7 +12327,7 @@
         <v>64.2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -11843,7 +12362,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -11878,7 +12397,7 @@
         <v>68.400000000000006</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -11913,7 +12432,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -11948,7 +12467,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -11983,7 +12502,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -12018,7 +12537,7 @@
         <v>60.4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -12053,7 +12572,7 @@
         <v>64.3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -12088,7 +12607,7 @@
         <v>60.3</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -12123,7 +12642,7 @@
         <v>51.8</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -12158,7 +12677,7 @@
         <v>64.099999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -12193,7 +12712,7 @@
         <v>76.7</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -12238,12 +12757,12 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12278,7 +12797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -12313,7 +12832,7 @@
         <v>474.4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -12348,7 +12867,7 @@
         <v>495.9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -12383,7 +12902,7 @@
         <v>501.3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -12418,7 +12937,7 @@
         <v>491.8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -12453,7 +12972,7 @@
         <v>468.6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -12488,7 +13007,7 @@
         <v>474.1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -12523,7 +13042,7 @@
         <v>479.6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -12558,7 +13077,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -12593,7 +13112,7 @@
         <v>447.7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -12628,7 +13147,7 @@
         <v>456.2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -12663,7 +13182,7 @@
         <v>466.8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -12698,7 +13217,7 @@
         <v>453.1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -12733,7 +13252,7 @@
         <v>440.3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -12768,7 +13287,7 @@
         <v>452.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -12803,7 +13322,7 @@
         <v>451.1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -12838,7 +13357,7 @@
         <v>450.9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -12873,7 +13392,7 @@
         <v>431.6</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -12908,7 +13427,7 @@
         <v>452.9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -12943,7 +13462,7 @@
         <v>462.6</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -12978,7 +13497,7 @@
         <v>453.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -13013,7 +13532,7 @@
         <v>438.1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -13048,7 +13567,7 @@
         <v>443.6</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -13083,7 +13602,7 @@
         <v>448.5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -13118,7 +13637,7 @@
         <v>447.8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -13153,7 +13672,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -13188,7 +13707,7 @@
         <v>451.6</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -13223,7 +13742,7 @@
         <v>456.3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -13258,7 +13777,7 @@
         <v>447.7</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -13293,7 +13812,7 @@
         <v>449.4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -13328,7 +13847,7 @@
         <v>455.1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -13363,7 +13882,7 @@
         <v>457.4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -13398,7 +13917,7 @@
         <v>453.7</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -13433,7 +13952,7 @@
         <v>464.3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -13468,7 +13987,7 @@
         <v>459.2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -13503,7 +14022,7 @@
         <v>467.4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -13538,7 +14057,7 @@
         <v>446.6</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -13573,7 +14092,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -13608,7 +14127,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -13643,7 +14162,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -13688,12 +14207,12 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13728,7 +14247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -13763,7 +14282,7 @@
         <v>362.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -13798,7 +14317,7 @@
         <v>369.1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -13833,7 +14352,7 @@
         <v>373.6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -13868,7 +14387,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -13903,7 +14422,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -13938,7 +14457,7 @@
         <v>352.3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -13973,7 +14492,7 @@
         <v>366.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -14008,7 +14527,7 @@
         <v>345.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -14043,7 +14562,7 @@
         <v>339.9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -14078,7 +14597,7 @@
         <v>357.8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -14113,7 +14632,7 @@
         <v>356.6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -14148,7 +14667,7 @@
         <v>347.8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -14183,7 +14702,7 @@
         <v>338.3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -14218,7 +14737,7 @@
         <v>346.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -14253,7 +14772,7 @@
         <v>345.9</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -14288,7 +14807,7 @@
         <v>334.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -14323,7 +14842,7 @@
         <v>327.7</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -14358,7 +14877,7 @@
         <v>319.3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -14393,7 +14912,7 @@
         <v>320.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -14428,7 +14947,7 @@
         <v>307.3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -14463,7 +14982,7 @@
         <v>293.89999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -14498,7 +15017,7 @@
         <v>299.8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -14533,7 +15052,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -14568,7 +15087,7 @@
         <v>283.7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -14603,7 +15122,7 @@
         <v>285.89999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -14638,7 +15157,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -14673,7 +15192,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -14708,7 +15227,7 @@
         <v>281.10000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -14743,7 +15262,7 @@
         <v>278.2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -14778,7 +15297,7 @@
         <v>281.5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -14813,7 +15332,7 @@
         <v>294.39999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -14848,7 +15367,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -14883,7 +15402,7 @@
         <v>275.3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -14918,7 +15437,7 @@
         <v>287.3</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -14953,7 +15472,7 @@
         <v>293.60000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -14988,7 +15507,7 @@
         <v>269.8</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -15023,7 +15542,7 @@
         <v>272.2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -15058,7 +15577,7 @@
         <v>266.39999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -15093,7 +15612,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>

</xml_diff>